<commit_message>
Update Leave Card 2/7/2024 3:30 PM
</commit_message>
<xml_diff>
--- a/CASUAL/LA SP-VMO/MARQUEZ, HENSLEY.xlsx
+++ b/CASUAL/LA SP-VMO/MARQUEZ, HENSLEY.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DOLE-PC\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA SP-VMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA SP-VMO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5425B64-6F04-4A13-B51D-AE4248356F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -358,7 +357,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -737,15 +736,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -758,11 +748,20 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1459,7 +1458,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1502,7 +1501,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1565,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1625,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1692,7 +1691,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1755,7 +1754,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1853,7 +1852,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1912,7 +1911,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1977,7 +1976,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2020,7 +2019,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2095,7 +2094,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2281,7 +2280,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2347,7 +2346,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2405,7 +2404,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2471,7 +2470,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2527,7 +2526,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2602,7 +2601,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2645,7 +2644,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2711,7 +2710,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2767,7 +2766,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2865,7 +2864,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2928,7 +2927,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2977,7 +2976,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2994,25 +2993,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A8:K139" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A8:K139" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="31">
+    <tableColumn id="1" name="PERIOD" dataDxfId="35"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="34"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="33"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="32"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="31">
       <calculatedColumnFormula>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="29">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="30"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="29">
       <calculatedColumnFormula>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="27">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="28"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="27">
       <calculatedColumnFormula>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="25"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="26"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3024,25 +3023,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K135" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K135" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="16">
+    <tableColumn id="1" name="PERIOD" dataDxfId="20"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="19"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="18"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="17"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="16">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="14">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="15"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="12">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="13"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="12">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="10"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="11"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3054,13 +3053,13 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="D2:G3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="D2:G3" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="D2:G3"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="DAYS"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="HOURS"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="MINUTES"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="EQUIVALENT HOURS" dataDxfId="5">
+    <tableColumn id="1" name="DAYS"/>
+    <tableColumn id="2" name="HOURS"/>
+    <tableColumn id="3" name="MINUTES"/>
+    <tableColumn id="4" name="EQUIVALENT HOURS" dataDxfId="5">
       <calculatedColumnFormula>SUMIFS(F7:F14,E7:E14,E3)+SUMIFS(D7:D66,C7:C66,F3)+D3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3069,14 +3068,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="J2:L3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="J2:L3" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="J2:L3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="DATE STARTED" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="LEAVE EARN" dataDxfId="1">
+    <tableColumn id="1" name="DATE STARTED" dataDxfId="2"/>
+    <tableColumn id="2" name="LEAVE EARN" dataDxfId="1">
       <calculatedColumnFormula>J4-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="LEAVE EARNED" dataDxfId="0">
+    <tableColumn id="3" name="LEAVE EARNED" dataDxfId="0">
       <calculatedColumnFormula>IF($J$4=1,1.25,IF(ISBLANK($J$3),"---",1.25-VLOOKUP($K$3,$I$8:$K$37,2)))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3380,7 +3379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3390,7 +3389,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3398,34 +3397,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="4056" topLeftCell="A84" activePane="bottomLeft"/>
+      <pane ySplit="4050" topLeftCell="A84" activePane="bottomLeft"/>
       <selection activeCell="F5" sqref="F5"/>
-      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
+      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -3437,16 +3436,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -3457,16 +3456,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="51"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="59"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -3477,18 +3476,18 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="55"/>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3496,7 +3495,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3509,24 +3508,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3561,7 +3560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3585,7 +3584,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>42</v>
       </c>
@@ -3607,7 +3606,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3627,7 +3626,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3647,7 +3646,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3667,7 +3666,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>43210</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3711,7 +3710,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -3731,7 +3730,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3751,7 +3750,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3771,7 +3770,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3791,7 +3790,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>43377</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3835,7 +3834,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3859,7 +3858,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>43</v>
       </c>
@@ -3877,7 +3876,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3897,7 +3896,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3917,7 +3916,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3937,7 +3936,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3957,7 +3956,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3977,7 +3976,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3997,7 +3996,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -4017,7 +4016,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -4037,7 +4036,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -4057,7 +4056,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -4077,7 +4076,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -4097,7 +4096,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -4121,7 +4120,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
         <v>44</v>
       </c>
@@ -4139,7 +4138,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -4159,7 +4158,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -4203,7 +4202,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -4223,7 +4222,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -4243,7 +4242,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -4263,7 +4262,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -4283,7 +4282,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -4303,7 +4302,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -4323,7 +4322,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -4343,7 +4342,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -4363,7 +4362,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -4387,7 +4386,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="48" t="s">
         <v>45</v>
       </c>
@@ -4405,7 +4404,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -4425,7 +4424,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -4445,7 +4444,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -4465,7 +4464,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -4485,7 +4484,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -4505,7 +4504,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -4525,7 +4524,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -4545,7 +4544,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -4565,7 +4564,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -4585,7 +4584,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -4605,7 +4604,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -4625,7 +4624,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -4649,7 +4648,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="48" t="s">
         <v>46</v>
       </c>
@@ -4667,7 +4666,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -4687,7 +4686,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -4707,7 +4706,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -4727,7 +4726,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
         <v>44652</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20" t="s">
         <v>100</v>
@@ -4773,7 +4772,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
         <v>44682</v>
       </c>
@@ -4797,7 +4796,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
         <v>44713</v>
       </c>
@@ -4821,7 +4820,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>44743</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>44762</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20" t="s">
         <v>95</v>
@@ -4867,7 +4866,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="49"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
         <v>44774</v>
       </c>
@@ -4887,7 +4886,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40">
         <v>44805</v>
       </c>
@@ -4913,7 +4912,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
       <c r="B74" s="20" t="s">
         <v>93</v>
@@ -4933,7 +4932,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40">
         <v>44835</v>
       </c>
@@ -4957,7 +4956,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
         <v>44866</v>
       </c>
@@ -4981,7 +4980,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
         <v>44896</v>
       </c>
@@ -5007,7 +5006,7 @@
         <v>44903</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20" t="s">
         <v>88</v>
@@ -5027,7 +5026,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="49"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
         <v>47</v>
       </c>
@@ -5045,7 +5044,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40">
         <v>44927</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>44973</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40">
         <v>44958</v>
       </c>
@@ -5091,7 +5090,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40">
         <v>44986</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>45002</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40">
         <v>45017</v>
       </c>
@@ -5137,7 +5136,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40">
         <v>45047</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>45065</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40">
         <v>45078</v>
       </c>
@@ -5183,7 +5182,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40">
         <v>45108</v>
       </c>
@@ -5209,7 +5208,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40">
         <v>45139</v>
       </c>
@@ -5229,7 +5228,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40">
         <v>45170</v>
       </c>
@@ -5249,7 +5248,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40">
         <v>45200</v>
       </c>
@@ -5269,7 +5268,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40">
         <v>45231</v>
       </c>
@@ -5289,7 +5288,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40">
         <v>45261</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="48" t="s">
         <v>102</v>
       </c>
@@ -5333,7 +5332,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40">
         <v>45322</v>
       </c>
@@ -5359,7 +5358,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40">
         <v>45323</v>
       </c>
@@ -5383,7 +5382,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40">
         <v>45352</v>
       </c>
@@ -5401,7 +5400,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40">
         <v>45383</v>
       </c>
@@ -5419,7 +5418,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40">
         <v>45413</v>
       </c>
@@ -5437,7 +5436,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40">
         <v>45444</v>
       </c>
@@ -5455,7 +5454,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40">
         <v>45474</v>
       </c>
@@ -5473,7 +5472,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40">
         <v>45505</v>
       </c>
@@ -5491,7 +5490,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40">
         <v>45536</v>
       </c>
@@ -5509,7 +5508,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40">
         <v>45566</v>
       </c>
@@ -5527,7 +5526,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40">
         <v>45597</v>
       </c>
@@ -5545,7 +5544,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40">
         <v>45627</v>
       </c>
@@ -5563,7 +5562,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40">
         <v>45658</v>
       </c>
@@ -5581,7 +5580,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40">
         <v>45689</v>
       </c>
@@ -5599,7 +5598,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40">
         <v>45717</v>
       </c>
@@ -5617,7 +5616,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40">
         <v>45748</v>
       </c>
@@ -5635,7 +5634,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40">
         <v>45778</v>
       </c>
@@ -5653,7 +5652,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40">
         <v>45809</v>
       </c>
@@ -5671,7 +5670,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40">
         <v>45839</v>
       </c>
@@ -5689,7 +5688,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5705,7 +5704,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5721,7 +5720,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5737,7 +5736,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5753,7 +5752,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5769,7 +5768,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5785,7 +5784,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5801,7 +5800,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5817,7 +5816,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5833,7 +5832,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5849,7 +5848,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5865,7 +5864,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5881,7 +5880,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5897,7 +5896,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5913,7 +5912,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5929,7 +5928,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5945,7 +5944,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5961,7 +5960,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5977,7 +5976,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5993,7 +5992,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -6009,7 +6008,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -6025,7 +6024,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -6041,7 +6040,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -6057,7 +6056,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="40"/>
       <c r="B135" s="20"/>
       <c r="C135" s="13"/>
@@ -6073,7 +6072,7 @@
       <c r="J135" s="11"/>
       <c r="K135" s="20"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="40"/>
       <c r="B136" s="20"/>
       <c r="C136" s="13"/>
@@ -6089,7 +6088,7 @@
       <c r="J136" s="11"/>
       <c r="K136" s="20"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="40"/>
       <c r="B137" s="20"/>
       <c r="C137" s="13"/>
@@ -6105,7 +6104,7 @@
       <c r="J137" s="11"/>
       <c r="K137" s="20"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="40"/>
       <c r="B138" s="20"/>
       <c r="C138" s="13"/>
@@ -6121,7 +6120,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="41"/>
       <c r="B139" s="15"/>
       <c r="C139" s="42"/>
@@ -6139,23 +6138,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6178,34 +6177,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K135"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="4056" topLeftCell="A27" activePane="bottomLeft"/>
+      <pane ySplit="4050" topLeftCell="A27" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
       <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -6218,16 +6217,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -6239,19 +6238,19 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57" t="str">
+      <c r="F3" s="54" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F3:G3),"---------",'2018 LEAVE CREDITS'!F3:G3)</f>
         <v>---------</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="59"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -6263,19 +6262,19 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="str">
+      <c r="F4" s="55" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v>SP</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="55"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J4" s="55"/>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -6283,7 +6282,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -6296,24 +6295,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -6348,7 +6347,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -6372,7 +6371,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>42</v>
       </c>
@@ -6394,7 +6393,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -6418,7 +6417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -6436,7 +6435,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -6454,7 +6453,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -6472,7 +6471,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -6496,7 +6495,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="15" t="s">
         <v>53</v>
@@ -6516,7 +6515,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="40">
         <v>43252</v>
       </c>
@@ -6538,7 +6537,7 @@
       <c r="J17" s="12"/>
       <c r="K17" s="15"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43282</v>
       </c>
@@ -6562,7 +6561,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
       <c r="B19" s="20" t="s">
         <v>57</v>
@@ -6582,7 +6581,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>43313</v>
       </c>
@@ -6606,7 +6605,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="20" t="s">
         <v>62</v>
@@ -6626,7 +6625,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>43344</v>
       </c>
@@ -6650,7 +6649,7 @@
         <v>43370</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="20" t="s">
         <v>61</v>
@@ -6670,7 +6669,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>43374</v>
       </c>
@@ -6694,7 +6693,7 @@
         <v>43397</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="20" t="s">
         <v>63</v>
@@ -6714,7 +6713,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>43405</v>
       </c>
@@ -6736,7 +6735,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>43435</v>
       </c>
@@ -6758,7 +6757,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="20" t="s">
         <v>65</v>
@@ -6778,7 +6777,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="48" t="s">
         <v>43</v>
       </c>
@@ -6796,7 +6795,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="40">
         <v>43497</v>
       </c>
@@ -6820,7 +6819,7 @@
         <v>43516</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>43556</v>
       </c>
@@ -6844,7 +6843,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="20" t="s">
         <v>54</v>
@@ -6866,7 +6865,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40">
         <v>43647</v>
       </c>
@@ -6890,7 +6889,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>43678</v>
       </c>
@@ -6914,7 +6913,7 @@
         <v>43691</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>43709</v>
       </c>
@@ -6938,7 +6937,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
         <v>43739</v>
       </c>
@@ -6962,7 +6961,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>43800</v>
       </c>
@@ -6986,7 +6985,7 @@
         <v>43825</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
         <v>44</v>
       </c>
@@ -7004,7 +7003,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>44013</v>
       </c>
@@ -7028,7 +7027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>44075</v>
       </c>
@@ -7052,7 +7051,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40"/>
       <c r="B41" s="20" t="s">
         <v>72</v>
@@ -7074,7 +7073,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
         <v>47</v>
       </c>
@@ -7092,7 +7091,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>44986</v>
       </c>
@@ -7116,7 +7115,7 @@
         <v>44986</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="40">
         <v>45047</v>
       </c>
@@ -7138,7 +7137,7 @@
         <v>45043</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>45110</v>
       </c>
@@ -7162,7 +7161,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>45170</v>
       </c>
@@ -7186,7 +7185,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>45200</v>
       </c>
@@ -7210,7 +7209,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>45231</v>
       </c>
@@ -7234,7 +7233,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -7250,7 +7249,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -7266,7 +7265,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -7282,7 +7281,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -7298,7 +7297,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -7314,7 +7313,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -7330,7 +7329,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -7346,7 +7345,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -7362,7 +7361,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -7378,7 +7377,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -7394,7 +7393,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -7410,7 +7409,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -7426,7 +7425,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -7442,7 +7441,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -7458,7 +7457,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -7474,7 +7473,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -7490,7 +7489,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -7506,7 +7505,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -7522,7 +7521,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -7538,7 +7537,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -7554,7 +7553,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -7570,7 +7569,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -7586,7 +7585,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -7602,7 +7601,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -7618,7 +7617,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -7634,7 +7633,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -7650,7 +7649,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -7666,7 +7665,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -7682,7 +7681,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -7698,7 +7697,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -7714,7 +7713,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -7730,7 +7729,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -7746,7 +7745,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -7762,7 +7761,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -7778,7 +7777,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -7794,7 +7793,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -7810,7 +7809,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -7826,7 +7825,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -7842,7 +7841,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -7858,7 +7857,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -7874,7 +7873,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -7890,7 +7889,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -7906,7 +7905,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -7922,7 +7921,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -7938,7 +7937,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -7954,7 +7953,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -7970,7 +7969,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -7986,7 +7985,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -8002,7 +8001,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -8018,7 +8017,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -8034,7 +8033,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -8050,7 +8049,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -8066,7 +8065,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -8082,7 +8081,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -8098,7 +8097,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -8114,7 +8113,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -8130,7 +8129,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -8146,7 +8145,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -8162,7 +8161,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -8178,7 +8177,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -8194,7 +8193,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -8210,7 +8209,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -8226,7 +8225,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -8242,7 +8241,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -8258,7 +8257,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -8274,7 +8273,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -8290,7 +8289,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -8306,7 +8305,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -8322,7 +8321,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -8338,7 +8337,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -8354,7 +8353,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -8370,7 +8369,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -8386,7 +8385,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -8402,7 +8401,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -8418,7 +8417,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -8434,7 +8433,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -8450,7 +8449,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -8466,7 +8465,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -8482,7 +8481,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -8498,7 +8497,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -8514,7 +8513,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -8530,7 +8529,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -8546,7 +8545,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -8562,7 +8561,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -8578,7 +8577,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -8594,7 +8593,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -8610,7 +8609,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="41"/>
       <c r="B135" s="15"/>
       <c r="C135" s="42"/>
@@ -8641,10 +8640,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8667,7 +8666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
@@ -8675,21 +8674,21 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="60" t="s">
         <v>33</v>
       </c>
@@ -8702,7 +8701,7 @@
       <c r="K1" s="61"/>
       <c r="L1" s="61"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -8731,7 +8730,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>51.709000000000003</v>
       </c>
@@ -8759,17 +8758,17 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -8790,7 +8789,7 @@
       <c r="K6" s="61"/>
       <c r="L6" s="61"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -8817,7 +8816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -8843,7 +8842,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -8869,7 +8868,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -8895,7 +8894,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -8921,7 +8920,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -8947,7 +8946,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -8973,7 +8972,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -8999,7 +8998,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -9019,7 +9018,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -9039,7 +9038,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -9059,7 +9058,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -9080,7 +9079,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -9101,7 +9100,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -9122,7 +9121,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -9143,7 +9142,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -9164,7 +9163,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -9185,7 +9184,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -9206,7 +9205,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -9227,7 +9226,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -9248,7 +9247,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -9269,7 +9268,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -9290,7 +9289,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -9311,7 +9310,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -9332,7 +9331,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -9353,7 +9352,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -9374,7 +9373,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -9395,7 +9394,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -9416,7 +9415,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -9437,7 +9436,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -9458,7 +9457,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -9479,7 +9478,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -9488,7 +9487,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -9497,7 +9496,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -9506,7 +9505,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -9515,7 +9514,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -9524,7 +9523,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -9533,7 +9532,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -9542,7 +9541,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -9551,7 +9550,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -9560,7 +9559,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -9569,7 +9568,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -9578,7 +9577,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -9587,7 +9586,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -9596,7 +9595,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -9605,7 +9604,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -9614,7 +9613,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -9623,7 +9622,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -9632,7 +9631,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -9641,7 +9640,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -9650,7 +9649,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -9659,7 +9658,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -9668,7 +9667,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -9677,7 +9676,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -9686,7 +9685,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -9695,7 +9694,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -9704,7 +9703,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -9713,7 +9712,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -9722,7 +9721,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -9731,7 +9730,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -9740,7 +9739,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>